<commit_message>
Some example for Task
</commit_message>
<xml_diff>
--- a/VariousExcercises/ReadingExcelFile/Files/QualitativeAssessmentTemplateSample.xlsx
+++ b/VariousExcercises/ReadingExcelFile/Files/QualitativeAssessmentTemplateSample.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
   <si>
     <t>Risk Category</t>
   </si>
@@ -105,6 +105,27 @@
   </si>
   <si>
     <t>Client Age Four # ImpactText = This Question about client age</t>
+  </si>
+  <si>
+    <t>Mitigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check if they paid </t>
+  </si>
+  <si>
+    <t>Hasn't be checked</t>
+  </si>
+  <si>
+    <t>They paid all previous amount</t>
+  </si>
+  <si>
+    <t>They paid some of previous amount</t>
+  </si>
+  <si>
+    <t>They did not paid</t>
+  </si>
+  <si>
+    <t>Mitigation Parameter</t>
   </si>
 </sst>
 </file>
@@ -140,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -151,6 +172,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -432,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,10 +470,10 @@
     <col min="4" max="4" width="72.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="73.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,8 +489,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -483,154 +513,159 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="2"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="3"/>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="2"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="3"/>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="5"/>
+      <c r="F6" s="3"/>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" s="3"/>
+      <c r="E7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="3"/>
-      <c r="C12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
       <c r="E12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" t="s">
-        <v>8</v>
+      <c r="E16" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
       <c r="E17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -639,7 +674,7 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -648,16 +683,22 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="1" t="s">
-        <v>19</v>
+      <c r="B20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -665,19 +706,17 @@
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" t="s">
-        <v>8</v>
+      <c r="E21" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="D22" s="3"/>
       <c r="E22" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -685,8 +724,8 @@
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" t="s">
-        <v>9</v>
+      <c r="E23" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -695,16 +734,18 @@
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="1" t="s">
-        <v>19</v>
+      <c r="D25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -713,20 +754,16 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="3"/>
-      <c r="C27" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
       <c r="E27" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -735,7 +772,7 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -744,16 +781,20 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="1" t="s">
-        <v>19</v>
+      <c r="C30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -761,19 +802,17 @@
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
-      <c r="E31" t="s">
-        <v>8</v>
+      <c r="E31" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
-      <c r="D32" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="D32" s="3"/>
       <c r="E32" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -781,8 +820,8 @@
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
-      <c r="E33" t="s">
-        <v>9</v>
+      <c r="E33" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -791,16 +830,18 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="1" t="s">
-        <v>19</v>
+      <c r="D35" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -809,25 +850,54 @@
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="D32:D36"/>
-    <mergeCell ref="B2:B16"/>
-    <mergeCell ref="B17:B36"/>
-    <mergeCell ref="A2:A36"/>
-    <mergeCell ref="D2:D6"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="C2:C11"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="D12:D16"/>
-    <mergeCell ref="C17:C26"/>
-    <mergeCell ref="D17:D21"/>
-    <mergeCell ref="D22:D26"/>
-    <mergeCell ref="C27:C36"/>
-    <mergeCell ref="D27:D31"/>
+  <mergeCells count="16">
+    <mergeCell ref="E3:E6"/>
+    <mergeCell ref="F3:F6"/>
+    <mergeCell ref="D35:D39"/>
+    <mergeCell ref="B2:B19"/>
+    <mergeCell ref="B20:B39"/>
+    <mergeCell ref="A2:A39"/>
+    <mergeCell ref="D2:D9"/>
+    <mergeCell ref="D10:D14"/>
+    <mergeCell ref="C2:C14"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="D15:D19"/>
+    <mergeCell ref="C20:C29"/>
+    <mergeCell ref="D20:D24"/>
+    <mergeCell ref="D25:D29"/>
+    <mergeCell ref="C30:C39"/>
+    <mergeCell ref="D30:D34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>